<commit_message>
cooling and ventilation data added (missing: cost and labor input data)
</commit_message>
<xml_diff>
--- a/projects/test_building/input/Parameter_CoolingTechnology_EfficiencyCoefficient.xlsx
+++ b/projects/test_building/input/Parameter_CoolingTechnology_EfficiencyCoefficient.xlsx
@@ -16,7 +16,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'lifetime_tuned (2)'!$A$1:$F$44</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -4614,7 +4614,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="191" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4648,7 +4648,7 @@
         <v>1</v>
       </c>
       <c r="D2">
-        <v>5</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -4662,7 +4662,7 @@
         <v>1</v>
       </c>
       <c r="D3">
-        <v>4.5</v>
+        <v>3.3</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -4676,7 +4676,7 @@
         <v>1</v>
       </c>
       <c r="D4">
-        <v>4</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -4690,7 +4690,7 @@
         <v>1</v>
       </c>
       <c r="D5">
-        <v>3.5</v>
+        <v>2.9</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -4704,7 +4704,7 @@
         <v>1</v>
       </c>
       <c r="D6">
-        <v>3</v>
+        <v>2.7</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -4732,7 +4732,7 @@
         <v>1</v>
       </c>
       <c r="D8">
-        <v>2</v>
+        <v>2.2999999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>